<commit_message>
download recent data remove star mark error check fix target
</commit_message>
<xml_diff>
--- a/result/back_testing_m3.xlsx
+++ b/result/back_testing_m3.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\kra3\result\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9405" yWindow="45" windowWidth="21000" windowHeight="9915" activeTab="1"/>
+    <workbookView xWindow="9408" yWindow="48" windowWidth="21000" windowHeight="9912" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -20,12 +15,12 @@
     <sheet name="4nw" sheetId="4" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="53">
   <si>
     <t>train data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -185,6 +180,18 @@
     <t>sum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>1등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -243,14 +250,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -314,7 +314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -349,7 +349,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,19 +564,19 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="4" width="6.25" customWidth="1"/>
-    <col min="5" max="5" width="7.75" customWidth="1"/>
-    <col min="6" max="13" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="25.09765625" customWidth="1"/>
+    <col min="3" max="4" width="6.19921875" customWidth="1"/>
+    <col min="5" max="5" width="7.69921875" customWidth="1"/>
+    <col min="6" max="13" width="6.19921875" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
-    <col min="16" max="16" width="6.25" customWidth="1"/>
-    <col min="17" max="17" width="7.75" customWidth="1"/>
-    <col min="18" max="25" width="6.25" customWidth="1"/>
+    <col min="16" max="16" width="6.19921875" customWidth="1"/>
+    <col min="17" max="17" width="7.69921875" customWidth="1"/>
+    <col min="18" max="25" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -600,7 +600,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -671,7 +671,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -773,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -782,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -791,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -836,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -854,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>25</v>
       </c>
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>27</v>
       </c>
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>28</v>
       </c>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>29</v>
       </c>
@@ -962,7 +962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>30</v>
       </c>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>33</v>
       </c>
@@ -998,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>35</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>36</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>37</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>38</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>39</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>40</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>41</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>42</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>43</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>44</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>45</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>46</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>47</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>48</v>
       </c>
@@ -1147,23 +1147,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="4" width="6.25" customWidth="1"/>
-    <col min="5" max="5" width="7.75" customWidth="1"/>
-    <col min="6" max="13" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="25.09765625" customWidth="1"/>
+    <col min="3" max="4" width="6.19921875" customWidth="1"/>
+    <col min="5" max="5" width="7.69921875" customWidth="1"/>
+    <col min="6" max="13" width="6.19921875" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
-    <col min="16" max="16" width="6.25" customWidth="1"/>
-    <col min="17" max="17" width="7.75" customWidth="1"/>
-    <col min="18" max="25" width="6.25" customWidth="1"/>
+    <col min="16" max="16" width="6.19921875" customWidth="1"/>
+    <col min="17" max="17" width="7.69921875" customWidth="1"/>
+    <col min="18" max="25" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -1187,7 +1187,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>-840</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>-764</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>8393</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>-856</v>
       </c>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>-309</v>
       </c>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>-1076</v>
       </c>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>-995</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>-910</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>-1088</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>13362</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>-770</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>25</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>3486</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>27</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>28</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>29</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>-787</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>30</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>-186</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>33</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>35</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>36</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>-1139</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>37</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>-1214</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>38</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>-1011</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>39</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>-1232</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>40</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>4517</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>41</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>5154</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>42</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>43</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>44</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>-644</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>45</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>46</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>-545</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>47</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>-950</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>48</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C47">
         <v>180</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C48">
         <v>817</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="49" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C49">
         <v>5332</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>5331</v>
       </c>
     </row>
-    <row r="50" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C50">
         <v>128</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C51">
         <v>790</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="52" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C52">
         <v>0</v>
       </c>
@@ -3309,7 +3309,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$N1&lt;&gt;$C1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3326,19 +3326,19 @@
       <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="4" width="6.25" customWidth="1"/>
-    <col min="5" max="5" width="7.75" customWidth="1"/>
-    <col min="6" max="13" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="25.09765625" customWidth="1"/>
+    <col min="3" max="4" width="6.19921875" customWidth="1"/>
+    <col min="5" max="5" width="7.69921875" customWidth="1"/>
+    <col min="6" max="13" width="6.19921875" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
-    <col min="16" max="16" width="6.25" customWidth="1"/>
-    <col min="17" max="17" width="7.75" customWidth="1"/>
-    <col min="18" max="25" width="6.25" customWidth="1"/>
+    <col min="16" max="16" width="6.19921875" customWidth="1"/>
+    <col min="17" max="17" width="7.69921875" customWidth="1"/>
+    <col min="18" max="25" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -3362,7 +3362,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>25</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>27</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>28</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>29</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>30</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>33</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>35</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>36</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>37</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>38</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>39</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>40</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>41</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>42</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>43</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>44</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>45</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>46</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>47</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>48</v>
       </c>
@@ -3912,13 +3912,13 @@
       <selection activeCell="B6" sqref="B6:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="13" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="25.09765625" customWidth="1"/>
+    <col min="3" max="13" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -3940,7 +3940,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -4027,207 +4027,207 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>48</v>
       </c>
@@ -4249,13 +4249,13 @@
       <selection activeCell="B6" sqref="B6:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="13" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="25.09765625" customWidth="1"/>
+    <col min="3" max="13" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -4277,7 +4277,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -4364,207 +4364,207 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>48</v>
       </c>
@@ -4587,13 +4587,13 @@
       <selection activeCell="B6" sqref="B6:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="13" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="25.09765625" customWidth="1"/>
+    <col min="3" max="13" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -4615,7 +4615,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -4702,207 +4702,207 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>48</v>
       </c>
@@ -4918,936 +4918,625 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="K1:P46"/>
+  <dimension ref="E1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K1">
-        <v>369</v>
-      </c>
-      <c r="L1">
-        <v>170</v>
-      </c>
-      <c r="M1">
-        <v>-450</v>
-      </c>
-      <c r="N1">
-        <v>-640</v>
-      </c>
-      <c r="O1">
-        <v>528</v>
-      </c>
-      <c r="P1">
+    <row r="1" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <f>SUM(E3:E101)</f>
+        <v>-4618</v>
+      </c>
+      <c r="F2">
+        <f>SUM(F3:F101)</f>
+        <v>41229</v>
+      </c>
+      <c r="G2">
+        <f>SUM(G3:G101)</f>
+        <v>-1348</v>
+      </c>
+    </row>
+    <row r="3" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>-1064</v>
+      </c>
+      <c r="F3">
+        <v>270</v>
+      </c>
+      <c r="G3">
+        <v>-656</v>
+      </c>
+    </row>
+    <row r="4" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1228</v>
+      </c>
+      <c r="F4">
+        <v>-840</v>
+      </c>
+      <c r="G4">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="5" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>-289</v>
+      </c>
+      <c r="F5">
+        <v>39</v>
+      </c>
+      <c r="G5">
+        <v>-834</v>
+      </c>
+    </row>
+    <row r="6" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>265</v>
+      </c>
+      <c r="F6">
+        <v>-764</v>
+      </c>
+      <c r="G6">
+        <v>-295</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>-1226</v>
+      </c>
+      <c r="F8">
+        <v>8373</v>
+      </c>
+      <c r="G8">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>103</v>
+      </c>
+      <c r="F9">
+        <v>-68</v>
+      </c>
+      <c r="G9">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="10" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>-426</v>
+      </c>
+      <c r="F10">
+        <v>1447</v>
+      </c>
+      <c r="G10">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="11" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>480</v>
+      </c>
+      <c r="F11">
+        <v>-856</v>
+      </c>
+      <c r="G11">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="12" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>-817</v>
+      </c>
+      <c r="F12">
+        <v>1148</v>
+      </c>
+      <c r="G12">
+        <v>-697</v>
+      </c>
+    </row>
+    <row r="13" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <v>-309</v>
+      </c>
+      <c r="G13">
+        <v>-751</v>
+      </c>
+    </row>
+    <row r="14" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>-995</v>
+      </c>
+      <c r="F15">
+        <v>-1076</v>
+      </c>
+      <c r="G15">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="16" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>-853</v>
+      </c>
+      <c r="F16">
+        <v>820</v>
+      </c>
+      <c r="G16">
+        <v>4395</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>151</v>
+      </c>
+      <c r="F17">
+        <v>-994</v>
+      </c>
+      <c r="G17">
+        <v>-1044</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>-879</v>
+      </c>
+      <c r="F18">
+        <v>232</v>
+      </c>
+      <c r="G18">
         <v>-1700</v>
       </c>
     </row>
-    <row r="2" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K2">
-        <v>-295</v>
-      </c>
-      <c r="L2">
-        <v>750</v>
-      </c>
-      <c r="M2">
-        <v>-90</v>
-      </c>
-      <c r="N2">
-        <v>-1310</v>
-      </c>
-      <c r="O2">
-        <v>460</v>
-      </c>
-      <c r="P2">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="3" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K3">
-        <v>-397</v>
-      </c>
-      <c r="L3">
-        <v>-340</v>
-      </c>
-      <c r="M3">
-        <v>780</v>
-      </c>
-      <c r="N3">
-        <v>-1110</v>
-      </c>
-      <c r="O3">
-        <v>1820</v>
-      </c>
-      <c r="P3">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="4" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K4">
-        <v>-764</v>
-      </c>
-      <c r="L4">
-        <v>-310</v>
-      </c>
-      <c r="M4">
-        <v>-1120</v>
-      </c>
-      <c r="N4">
-        <v>580</v>
-      </c>
-      <c r="O4">
-        <v>-970</v>
-      </c>
-      <c r="P4">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="5" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K5">
-        <v>8067</v>
-      </c>
-      <c r="L5">
-        <v>-540</v>
-      </c>
-      <c r="M5">
-        <v>-990</v>
-      </c>
-      <c r="N5">
-        <v>-860</v>
-      </c>
-      <c r="O5">
-        <v>-2200</v>
-      </c>
-      <c r="P5">
-        <v>-2200</v>
-      </c>
-    </row>
-    <row r="6" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K6">
-        <v>2689</v>
-      </c>
-      <c r="L6">
-        <v>370</v>
-      </c>
-      <c r="M6">
-        <v>-220</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>-1220</v>
-      </c>
-      <c r="P6">
+    <row r="19" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>852</v>
+      </c>
+      <c r="F19">
+        <v>-910</v>
+      </c>
+      <c r="G19">
+        <v>-991</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>-688</v>
+      </c>
+      <c r="F20">
+        <v>-1088</v>
+      </c>
+      <c r="G20">
+        <v>-1322</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>605</v>
+      </c>
+      <c r="F21">
+        <v>13323</v>
+      </c>
+      <c r="G21">
+        <v>4370</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>-384</v>
+      </c>
+      <c r="F22">
         <v>-770</v>
       </c>
-    </row>
-    <row r="7" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K7">
-        <v>-856</v>
-      </c>
-      <c r="L7">
-        <v>-390</v>
-      </c>
-      <c r="M7">
-        <v>3396</v>
-      </c>
-      <c r="N7">
-        <v>364</v>
-      </c>
-      <c r="O7">
-        <v>-240</v>
-      </c>
-      <c r="P7">
+      <c r="G22">
+        <v>2545</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>-715</v>
+      </c>
+      <c r="F23">
+        <v>3059</v>
+      </c>
+      <c r="G23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E24">
         <v>-1600</v>
       </c>
-    </row>
-    <row r="8" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K8">
+      <c r="F24">
+        <v>638</v>
+      </c>
+      <c r="G24">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>77</v>
+      </c>
+      <c r="F25">
+        <v>442</v>
+      </c>
+      <c r="G25">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>-835</v>
+      </c>
+      <c r="F26">
+        <v>1005</v>
+      </c>
+      <c r="G26">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>-635</v>
+      </c>
+      <c r="F27">
+        <v>-787</v>
+      </c>
+      <c r="G27">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E28">
+        <v>-362</v>
+      </c>
+      <c r="F28">
+        <v>-186</v>
+      </c>
+      <c r="G28">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E29">
+        <v>1599</v>
+      </c>
+      <c r="F29">
+        <v>217</v>
+      </c>
+      <c r="G29">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E30">
+        <v>-944</v>
+      </c>
+      <c r="F30">
+        <v>1912</v>
+      </c>
+      <c r="G30">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E31">
+        <v>-261</v>
+      </c>
+      <c r="F31">
+        <v>1189</v>
+      </c>
+      <c r="G31">
+        <v>-916</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E32">
+        <v>-963</v>
+      </c>
+      <c r="F32">
+        <v>1324</v>
+      </c>
+      <c r="G32">
+        <v>-989</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E33">
+        <v>820</v>
+      </c>
+      <c r="F33">
+        <v>856</v>
+      </c>
+      <c r="G33">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E34">
+        <v>-956</v>
+      </c>
+      <c r="F34">
+        <v>-1139</v>
+      </c>
+      <c r="G34">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E35">
+        <v>1289</v>
+      </c>
+      <c r="F35">
+        <v>-1214</v>
+      </c>
+      <c r="G35">
+        <v>-471</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E36">
+        <v>-493</v>
+      </c>
+      <c r="F36">
+        <v>-1011</v>
+      </c>
+      <c r="G36">
+        <v>-1292</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E37">
+        <v>-532</v>
+      </c>
+      <c r="F37">
+        <v>-1232</v>
+      </c>
+      <c r="G37">
+        <v>-1164</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E38">
+        <v>-697</v>
+      </c>
+      <c r="F38">
+        <v>4497</v>
+      </c>
+      <c r="G38">
+        <v>-58</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E40">
+        <v>3624</v>
+      </c>
+      <c r="F40">
+        <v>-740</v>
+      </c>
+      <c r="G40">
+        <v>-763</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E41">
+        <v>459</v>
+      </c>
+      <c r="F41">
+        <v>5134</v>
+      </c>
+      <c r="G41">
+        <v>-653</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E42">
+        <v>-446</v>
+      </c>
+      <c r="F42">
+        <v>424</v>
+      </c>
+      <c r="G42">
+        <v>-1800</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E43">
+        <v>1048</v>
+      </c>
+      <c r="F43">
+        <v>670</v>
+      </c>
+      <c r="G43">
+        <v>-1541</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E44">
+        <v>1588</v>
+      </c>
+      <c r="F44">
+        <v>-644</v>
+      </c>
+      <c r="G44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E45">
+        <v>-234</v>
+      </c>
+      <c r="F45">
+        <v>2111</v>
+      </c>
+      <c r="G45">
+        <v>-410</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E47">
+        <v>359</v>
+      </c>
+      <c r="F47">
+        <v>-545</v>
+      </c>
+      <c r="G47">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E48">
+        <v>-39</v>
+      </c>
+      <c r="F48">
+        <v>-949</v>
+      </c>
+      <c r="G48">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E49">
+        <v>-1023</v>
+      </c>
+      <c r="F49">
         <v>1435</v>
       </c>
-      <c r="L8">
-        <v>200</v>
-      </c>
-      <c r="M8">
-        <v>4350</v>
-      </c>
-      <c r="N8">
-        <v>-90</v>
-      </c>
-      <c r="O8">
-        <v>-1800</v>
-      </c>
-      <c r="P8">
-        <v>-1800</v>
-      </c>
-    </row>
-    <row r="9" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K9">
-        <v>-309</v>
-      </c>
-      <c r="L9">
-        <v>-450</v>
-      </c>
-      <c r="M9">
-        <v>-170</v>
-      </c>
-      <c r="N9">
-        <v>-1600</v>
-      </c>
-      <c r="O9">
-        <v>-1290</v>
-      </c>
-      <c r="P9">
-        <v>-1360</v>
-      </c>
-    </row>
-    <row r="10" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K10">
-        <v>-1631</v>
-      </c>
-      <c r="L10">
-        <v>-660</v>
-      </c>
-      <c r="M10">
-        <v>-820</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>-450</v>
-      </c>
-      <c r="P10">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="11" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K11">
-        <v>781</v>
-      </c>
-      <c r="L11">
-        <v>-50</v>
-      </c>
-      <c r="M11">
-        <v>-1490</v>
-      </c>
-      <c r="N11">
-        <v>-1700</v>
-      </c>
-      <c r="O11">
-        <v>-1210</v>
-      </c>
-      <c r="P11">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="12" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K12">
-        <v>-865</v>
-      </c>
-      <c r="L12">
-        <v>60</v>
-      </c>
-      <c r="M12">
-        <v>-770</v>
-      </c>
-      <c r="N12">
-        <v>-1120</v>
-      </c>
-      <c r="O12">
-        <v>-250</v>
-      </c>
-      <c r="P12">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="13" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K13">
-        <v>-811</v>
-      </c>
-      <c r="L13">
-        <v>-510</v>
-      </c>
-      <c r="M13">
-        <v>-760</v>
-      </c>
-      <c r="N13">
-        <v>-1700</v>
-      </c>
-      <c r="O13">
-        <v>-1700</v>
-      </c>
-      <c r="P13">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="14" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K14">
-        <v>-910</v>
-      </c>
-      <c r="L14">
-        <v>-330</v>
-      </c>
-      <c r="M14">
-        <v>590</v>
-      </c>
-      <c r="N14">
-        <v>-1090</v>
-      </c>
-      <c r="O14">
-        <v>640</v>
-      </c>
-      <c r="P14">
-        <v>-700</v>
-      </c>
-    </row>
-    <row r="15" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K15">
-        <v>1134</v>
-      </c>
-      <c r="L15">
-        <v>70</v>
-      </c>
-      <c r="M15">
-        <v>-980</v>
-      </c>
-      <c r="N15">
-        <v>-1600</v>
-      </c>
-      <c r="O15">
-        <v>-1600</v>
-      </c>
-      <c r="P15">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="16" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K16">
-        <v>11478</v>
-      </c>
-      <c r="L16">
-        <v>540</v>
-      </c>
-      <c r="M16">
-        <v>-820</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>-1800</v>
-      </c>
-      <c r="P16">
-        <v>-1800</v>
-      </c>
-    </row>
-    <row r="17" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K17">
-        <v>-441</v>
-      </c>
-      <c r="L17">
-        <v>140</v>
-      </c>
-      <c r="M17">
-        <v>1940</v>
-      </c>
-      <c r="N17">
-        <v>-250</v>
-      </c>
-      <c r="O17">
-        <v>-340</v>
-      </c>
-      <c r="P17">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="18" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K18">
-        <v>1450</v>
-      </c>
-      <c r="L18">
-        <v>-60</v>
-      </c>
-      <c r="M18">
-        <v>-1290</v>
-      </c>
-      <c r="N18">
-        <v>-1230</v>
-      </c>
-      <c r="O18">
-        <v>-1220</v>
-      </c>
-      <c r="P18">
-        <v>-1240</v>
-      </c>
-    </row>
-    <row r="19" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K19">
-        <v>559</v>
-      </c>
-      <c r="L19">
-        <v>-270</v>
-      </c>
-      <c r="M19">
-        <v>-960</v>
-      </c>
-      <c r="N19">
-        <v>370</v>
-      </c>
-      <c r="O19">
-        <v>-1600</v>
-      </c>
-      <c r="P19">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="20" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K20">
-        <v>-56</v>
-      </c>
-      <c r="L20">
-        <v>-570</v>
-      </c>
-      <c r="M20">
-        <v>-1050</v>
-      </c>
-      <c r="N20">
-        <v>870</v>
-      </c>
-      <c r="O20">
-        <v>-1100</v>
-      </c>
-      <c r="P20">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="21" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K21">
-        <v>1423</v>
-      </c>
-      <c r="L21">
-        <v>-350</v>
-      </c>
-      <c r="M21">
-        <v>-840</v>
-      </c>
-      <c r="N21">
-        <v>232</v>
-      </c>
-      <c r="O21">
-        <v>-1140</v>
-      </c>
-      <c r="P21">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="22" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K22">
-        <v>-787</v>
-      </c>
-      <c r="L22">
-        <v>-350</v>
-      </c>
-      <c r="M22">
-        <v>160</v>
-      </c>
-      <c r="N22">
-        <v>-1130</v>
-      </c>
-      <c r="O22">
-        <v>2070</v>
-      </c>
-      <c r="P22">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="23" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K23">
-        <v>4184</v>
-      </c>
-      <c r="L23">
-        <v>110</v>
-      </c>
-      <c r="M23">
-        <v>-1600</v>
-      </c>
-      <c r="N23">
-        <v>-1600</v>
-      </c>
-      <c r="O23">
-        <v>-1600</v>
-      </c>
-      <c r="P23">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="24" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K24">
-        <v>363</v>
-      </c>
-      <c r="L24">
-        <v>400</v>
-      </c>
-      <c r="M24">
-        <v>-700</v>
-      </c>
-      <c r="N24">
-        <v>-1270</v>
-      </c>
-      <c r="O24">
-        <v>-640</v>
-      </c>
-      <c r="P24">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="25" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K25">
-        <v>610</v>
-      </c>
-      <c r="L25">
-        <v>-120</v>
-      </c>
-      <c r="M25">
-        <v>-1390</v>
-      </c>
-      <c r="N25">
-        <v>3710</v>
-      </c>
-      <c r="O25">
-        <v>-1600</v>
-      </c>
-      <c r="P25">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="26" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K26">
-        <v>980</v>
-      </c>
-      <c r="L26">
-        <v>-330</v>
-      </c>
-      <c r="M26">
-        <v>510</v>
-      </c>
-      <c r="N26">
-        <v>480</v>
-      </c>
-      <c r="O26">
-        <v>-1030</v>
-      </c>
-      <c r="P26">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="27" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K27">
-        <v>2706</v>
-      </c>
-      <c r="L27">
-        <v>-450</v>
-      </c>
-      <c r="M27">
-        <v>-1360</v>
-      </c>
-      <c r="N27">
-        <v>-100</v>
-      </c>
-      <c r="O27">
-        <v>-1220</v>
-      </c>
-      <c r="P27">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="28" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K28">
-        <v>876</v>
-      </c>
-      <c r="L28">
-        <v>-510</v>
-      </c>
-      <c r="M28">
-        <v>-880</v>
-      </c>
-      <c r="N28">
-        <v>-1070</v>
-      </c>
-      <c r="O28">
-        <v>-470</v>
-      </c>
-      <c r="P28">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="29" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K29">
-        <v>-718</v>
-      </c>
-      <c r="L29">
-        <v>540</v>
-      </c>
-      <c r="M29">
-        <v>-1420</v>
-      </c>
-      <c r="N29">
-        <v>-1600</v>
-      </c>
-      <c r="O29">
-        <v>-1600</v>
-      </c>
-      <c r="P29">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="30" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K30">
-        <v>-1600</v>
-      </c>
-      <c r="L30">
-        <v>1050</v>
-      </c>
-      <c r="M30">
-        <v>-1600</v>
-      </c>
-      <c r="N30">
-        <v>550</v>
-      </c>
-      <c r="O30">
-        <v>-1600</v>
-      </c>
-      <c r="P30">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="31" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K31">
-        <v>-523</v>
-      </c>
-      <c r="L31">
-        <v>-370</v>
-      </c>
-      <c r="M31">
-        <v>-1700</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>-1700</v>
-      </c>
-      <c r="P31">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="32" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K32">
-        <v>119</v>
-      </c>
-      <c r="L32">
-        <v>10</v>
-      </c>
-      <c r="M32">
-        <v>-1600</v>
-      </c>
-      <c r="N32">
-        <v>-710</v>
-      </c>
-      <c r="O32">
-        <v>-1600</v>
-      </c>
-      <c r="P32">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="33" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K33">
-        <v>3441</v>
-      </c>
-      <c r="L33">
-        <v>130</v>
-      </c>
-      <c r="M33">
-        <v>1846</v>
-      </c>
-      <c r="N33">
-        <v>-920</v>
-      </c>
-      <c r="O33">
-        <v>15902</v>
-      </c>
-      <c r="P33">
-        <v>-1140</v>
-      </c>
-    </row>
-    <row r="34" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K34">
-        <v>-437</v>
-      </c>
-      <c r="L34">
-        <v>30</v>
-      </c>
-      <c r="M34">
-        <v>-270</v>
-      </c>
-      <c r="N34">
-        <v>580</v>
-      </c>
-      <c r="O34">
-        <v>-370</v>
-      </c>
-      <c r="P34">
-        <v>-1800</v>
-      </c>
-    </row>
-    <row r="35" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K35">
-        <v>-1413</v>
-      </c>
-      <c r="L35">
-        <v>-710</v>
-      </c>
-      <c r="M35">
-        <v>182</v>
-      </c>
-      <c r="N35">
-        <v>486</v>
-      </c>
-      <c r="O35">
-        <v>-1690</v>
-      </c>
-      <c r="P35">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="36" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K36">
-        <v>1668</v>
-      </c>
-      <c r="L36">
-        <v>-410</v>
-      </c>
-      <c r="M36">
-        <v>1190</v>
-      </c>
-      <c r="N36">
-        <v>2080</v>
-      </c>
-      <c r="O36">
-        <v>1606</v>
-      </c>
-      <c r="P36">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="37" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K37">
-        <v>157</v>
-      </c>
-      <c r="L37">
-        <v>-160</v>
-      </c>
-      <c r="M37">
-        <v>1582</v>
-      </c>
-      <c r="N37">
-        <v>-1590</v>
-      </c>
-      <c r="O37">
-        <v>-1800</v>
-      </c>
-      <c r="P37">
-        <v>-1800</v>
-      </c>
-    </row>
-    <row r="38" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K38">
-        <v>-228</v>
-      </c>
-      <c r="L38">
-        <v>280</v>
-      </c>
-      <c r="M38">
-        <v>-1320</v>
-      </c>
-      <c r="N38">
-        <v>-1600</v>
-      </c>
-      <c r="O38">
-        <v>-1260</v>
-      </c>
-      <c r="P38">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="39" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K39">
-        <v>-224</v>
-      </c>
-      <c r="L39">
-        <v>740</v>
-      </c>
-      <c r="M39">
-        <v>3740</v>
-      </c>
-      <c r="N39">
-        <v>228</v>
-      </c>
-      <c r="O39">
-        <v>2450</v>
-      </c>
-      <c r="P39">
-        <v>-920</v>
-      </c>
-    </row>
-    <row r="40" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K40">
-        <v>2090</v>
-      </c>
-      <c r="L40">
-        <v>-460</v>
-      </c>
-      <c r="M40">
-        <v>-760</v>
-      </c>
-      <c r="N40">
-        <v>-1290</v>
-      </c>
-      <c r="O40">
-        <v>-1150</v>
-      </c>
-      <c r="P40">
-        <v>-1220</v>
-      </c>
-    </row>
-    <row r="41" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K41">
-        <v>-943</v>
-      </c>
-      <c r="L41">
-        <v>-270</v>
-      </c>
-      <c r="M41">
-        <v>-1600</v>
-      </c>
-      <c r="N41">
-        <v>-1140</v>
-      </c>
-      <c r="O41">
-        <v>-1600</v>
-      </c>
-      <c r="P41">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="42" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K42">
-        <v>736</v>
-      </c>
-      <c r="L42">
-        <v>-510</v>
-      </c>
-      <c r="M42">
-        <v>-10</v>
-      </c>
-      <c r="N42">
-        <v>-1600</v>
-      </c>
-      <c r="O42">
-        <v>-1070</v>
-      </c>
-      <c r="P42">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="43" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K43">
+      <c r="G49">
+        <v>-1114</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E50">
+        <v>1629</v>
+      </c>
+      <c r="F50">
+        <v>180</v>
+      </c>
+      <c r="G50">
+        <v>-1141</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E51">
+        <v>-35</v>
+      </c>
+      <c r="F51">
         <v>817</v>
       </c>
-      <c r="L43">
-        <v>-140</v>
-      </c>
-      <c r="M43">
-        <v>870</v>
-      </c>
-      <c r="N43">
-        <v>-950</v>
-      </c>
-      <c r="O43">
-        <v>60</v>
-      </c>
-      <c r="P43">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="44" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K44">
-        <v>5667</v>
-      </c>
-      <c r="L44">
-        <v>640</v>
-      </c>
-      <c r="M44">
-        <v>13374</v>
-      </c>
-      <c r="N44">
-        <v>-810</v>
-      </c>
-      <c r="O44">
-        <v>-1700</v>
-      </c>
-      <c r="P44">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="45" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K45">
-        <v>-438</v>
-      </c>
-      <c r="L45">
-        <v>-100</v>
-      </c>
-      <c r="M45">
-        <v>-830</v>
-      </c>
-      <c r="N45">
-        <v>-50</v>
-      </c>
-      <c r="O45">
-        <v>-180</v>
-      </c>
-      <c r="P45">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="46" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K46">
-        <v>1281</v>
-      </c>
-      <c r="L46">
-        <v>-510</v>
-      </c>
-      <c r="M46">
-        <v>-1700</v>
-      </c>
-      <c r="N46">
-        <v>-1550</v>
-      </c>
-      <c r="O46">
-        <v>-1700</v>
-      </c>
-      <c r="P46">
-        <v>-1700</v>
+      <c r="G51">
+        <v>-999</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E52">
+        <v>-798</v>
+      </c>
+      <c r="F52">
+        <v>5272</v>
+      </c>
+      <c r="G52">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E53">
+        <v>-526</v>
+      </c>
+      <c r="F53">
+        <v>128</v>
+      </c>
+      <c r="G53">
+        <v>-1330</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E54">
+        <v>-1122</v>
+      </c>
+      <c r="F54">
+        <v>389</v>
+      </c>
+      <c r="G54">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add recent data, backtesting
</commit_message>
<xml_diff>
--- a/result/back_testing_m3.xlsx
+++ b/result/back_testing_m3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12975" yWindow="45" windowWidth="21000" windowHeight="9915" activeTab="4"/>
+    <workbookView xWindow="16545" yWindow="45" windowWidth="21000" windowHeight="9915" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="y1_t0" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
     <sheet name="y4_t0" sheetId="2" r:id="rId3"/>
     <sheet name="sambok" sheetId="8" r:id="rId4"/>
     <sheet name="strategy" sheetId="9" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="68">
   <si>
     <t>2016-01-08 - 2016-01-10</t>
   </si>
@@ -236,6 +236,18 @@
     <t>total bet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>sun only</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3top2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -244,7 +256,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +273,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -291,7 +312,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -305,6 +326,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -12947,10 +12971,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12958,7 +12982,7 @@
     <col min="11" max="12" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -12996,8 +13020,11 @@
         <f>1+L52/(J1*1000)</f>
         <v>1.32717</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>57</v>
       </c>
@@ -13015,6 +13042,9 @@
       </c>
       <c r="G2" t="s">
         <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
       </c>
       <c r="I2" t="s">
         <v>63</v>
@@ -13023,8 +13053,32 @@
         <f>SUM(B3:G3)</f>
         <v>196302</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B3">
         <f>SUM(B4:B101)</f>
         <v>51088</v>
@@ -13049,8 +13103,40 @@
         <f t="shared" si="1"/>
         <v>41152</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P3">
+        <f>SUM(P4:P101)</f>
+        <v>19460</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:V3" si="2">SUM(Q4:Q101)</f>
+        <v>1979</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="2"/>
+        <v>25906</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="2"/>
+        <v>5798</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="2"/>
+        <v>25332</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="2"/>
+        <v>16211</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="2"/>
+        <v>8519</v>
+      </c>
+      <c r="W3">
+        <f>SUM(P3:U3)</f>
+        <v>94686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3467</v>
       </c>
@@ -13073,8 +13159,33 @@
         <f>SUM(B4:G4)/6*2</f>
         <v>-617.33333333333337</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>494</v>
+      </c>
+      <c r="Q4">
+        <v>167</v>
+      </c>
+      <c r="R4">
+        <v>-91</v>
+      </c>
+      <c r="S4">
+        <v>1966</v>
+      </c>
+      <c r="T4">
+        <v>-171</v>
+      </c>
+      <c r="U4">
+        <v>1190</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4:W51" si="3">SUM(P4:U4)</f>
+        <v>3555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1175</v>
       </c>
@@ -13094,15 +13205,40 @@
         <v>4682</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" ref="K5:K52" si="2">SUM(B5:G5)/6*2</f>
+        <f t="shared" ref="K5:K52" si="4">SUM(B5:G5)/6*2</f>
         <v>4122</v>
       </c>
       <c r="L5" s="4">
         <f>SUM(K$4:K5)</f>
         <v>3504.6666666666665</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>765</v>
+      </c>
+      <c r="Q5">
+        <v>107</v>
+      </c>
+      <c r="R5">
+        <v>-600</v>
+      </c>
+      <c r="S5">
+        <v>160</v>
+      </c>
+      <c r="T5">
+        <v>-600</v>
+      </c>
+      <c r="U5">
+        <v>1971</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="3"/>
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>-335</v>
       </c>
@@ -13122,15 +13258,40 @@
         <v>871</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1346.6666666666667</v>
       </c>
       <c r="L6" s="4">
         <f>SUM(K$4:K6)</f>
         <v>2158</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>614</v>
+      </c>
+      <c r="Q6">
+        <v>-281</v>
+      </c>
+      <c r="R6">
+        <v>-600</v>
+      </c>
+      <c r="S6">
+        <v>-600</v>
+      </c>
+      <c r="T6">
+        <v>-600</v>
+      </c>
+      <c r="U6">
+        <v>-454</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="3"/>
+        <v>-1921</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>-486</v>
       </c>
@@ -13150,15 +13311,40 @@
         <v>-1274</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1845.3333333333333</v>
       </c>
       <c r="L7" s="4">
         <f>SUM(K$4:K7)</f>
         <v>312.66666666666674</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>7221</v>
+      </c>
+      <c r="Q7">
+        <v>-623</v>
+      </c>
+      <c r="R7">
+        <v>2066</v>
+      </c>
+      <c r="S7">
+        <v>-680</v>
+      </c>
+      <c r="T7">
+        <v>1760</v>
+      </c>
+      <c r="U7">
+        <v>718</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="3"/>
+        <v>10462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>8550</v>
       </c>
@@ -13178,15 +13364,40 @@
         <v>100</v>
       </c>
       <c r="K8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3305.6666666666665</v>
       </c>
       <c r="L8" s="4">
         <f>SUM(K$4:K8)</f>
         <v>3618.333333333333</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>121</v>
+      </c>
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>-600</v>
+      </c>
+      <c r="S8">
+        <v>-80</v>
+      </c>
+      <c r="T8">
+        <v>-600</v>
+      </c>
+      <c r="U8">
+        <v>-600</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="3"/>
+        <v>-1751</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>121</v>
       </c>
@@ -13206,15 +13417,40 @@
         <v>-600</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-583.66666666666663</v>
       </c>
       <c r="L9" s="4">
         <f>SUM(K$4:K9)</f>
         <v>3034.6666666666665</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>11</v>
+      </c>
+      <c r="Q9">
+        <v>247</v>
+      </c>
+      <c r="R9">
+        <v>-600</v>
+      </c>
+      <c r="S9">
+        <v>-600</v>
+      </c>
+      <c r="T9">
+        <v>-600</v>
+      </c>
+      <c r="U9">
+        <v>974</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="3"/>
+        <v>-568</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1054</v>
       </c>
@@ -13234,15 +13470,40 @@
         <v>1606</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2866.6666666666665</v>
       </c>
       <c r="L10" s="4">
         <f>SUM(K$4:K10)</f>
         <v>5901.333333333333</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>-600</v>
+      </c>
+      <c r="Q10">
+        <v>118</v>
+      </c>
+      <c r="R10">
+        <v>-21</v>
+      </c>
+      <c r="S10">
+        <v>1440</v>
+      </c>
+      <c r="T10">
+        <v>-87</v>
+      </c>
+      <c r="U10">
+        <v>-200</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="3"/>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>808</v>
       </c>
@@ -13262,15 +13523,40 @@
         <v>-1200</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1116</v>
       </c>
       <c r="L11" s="4">
         <f>SUM(K$4:K11)</f>
         <v>7017.333333333333</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>-371</v>
+      </c>
+      <c r="Q11">
+        <v>-72</v>
+      </c>
+      <c r="R11">
+        <v>-600</v>
+      </c>
+      <c r="S11">
+        <v>-600</v>
+      </c>
+      <c r="T11">
+        <v>-600</v>
+      </c>
+      <c r="U11">
+        <v>-506</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="3"/>
+        <v>-2749</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>-238</v>
       </c>
@@ -13290,15 +13576,40 @@
         <v>1394</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>740</v>
       </c>
       <c r="L12" s="4">
         <f>SUM(K$4:K12)</f>
         <v>7757.333333333333</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>-600</v>
+      </c>
+      <c r="Q12">
+        <v>1023</v>
+      </c>
+      <c r="R12">
+        <v>4116</v>
+      </c>
+      <c r="S12">
+        <v>-330</v>
+      </c>
+      <c r="T12">
+        <v>7120</v>
+      </c>
+      <c r="U12">
+        <v>-600</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="3"/>
+        <v>10729</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>-1411</v>
       </c>
@@ -13318,15 +13629,40 @@
         <v>882</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2959.3333333333335</v>
       </c>
       <c r="L13" s="4">
         <f>SUM(K$4:K13)</f>
         <v>10716.666666666666</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <v>-580</v>
+      </c>
+      <c r="Q13">
+        <v>919</v>
+      </c>
+      <c r="R13">
+        <v>1470</v>
+      </c>
+      <c r="S13">
+        <v>240</v>
+      </c>
+      <c r="T13">
+        <v>983</v>
+      </c>
+      <c r="U13">
+        <v>-600</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="3"/>
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>-1432</v>
       </c>
@@ -13346,15 +13682,40 @@
         <v>-1520</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>461.33333333333331</v>
       </c>
       <c r="L14" s="4">
         <f>SUM(K$4:K14)</f>
         <v>11178</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>-194</v>
+      </c>
+      <c r="Q14">
+        <v>37</v>
+      </c>
+      <c r="R14">
+        <v>7046</v>
+      </c>
+      <c r="S14">
+        <v>1934</v>
+      </c>
+      <c r="T14">
+        <v>7504</v>
+      </c>
+      <c r="U14">
+        <v>1328</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="3"/>
+        <v>17655</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>3142</v>
       </c>
@@ -13374,15 +13735,40 @@
         <v>8021</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10528</v>
       </c>
       <c r="L15" s="4">
         <f>SUM(K$4:K15)</f>
         <v>21706</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>-262</v>
+      </c>
+      <c r="Q15">
+        <v>19</v>
+      </c>
+      <c r="R15">
+        <v>-500</v>
+      </c>
+      <c r="S15">
+        <v>-200</v>
+      </c>
+      <c r="T15">
+        <v>-500</v>
+      </c>
+      <c r="U15">
+        <v>-500</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="3"/>
+        <v>-1943</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>-1174</v>
       </c>
@@ -13402,15 +13788,40 @@
         <v>-1406</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1643.3333333333333</v>
       </c>
       <c r="L16" s="4">
         <f>SUM(K$4:K16)</f>
         <v>20062.666666666668</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>-600</v>
+      </c>
+      <c r="Q16">
+        <v>312</v>
+      </c>
+      <c r="R16">
+        <v>-600</v>
+      </c>
+      <c r="S16">
+        <v>-400</v>
+      </c>
+      <c r="T16">
+        <v>-600</v>
+      </c>
+      <c r="U16">
+        <v>398</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="3"/>
+        <v>-1490</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>-125</v>
       </c>
@@ -13430,15 +13841,40 @@
         <v>-158</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1651.6666666666667</v>
       </c>
       <c r="L17" s="4">
         <f>SUM(K$4:K17)</f>
         <v>18411</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>-600</v>
+      </c>
+      <c r="Q17">
+        <v>210</v>
+      </c>
+      <c r="R17">
+        <v>-600</v>
+      </c>
+      <c r="S17">
+        <v>-470</v>
+      </c>
+      <c r="T17">
+        <v>-600</v>
+      </c>
+      <c r="U17">
+        <v>-486</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="3"/>
+        <v>-2546</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>-189</v>
       </c>
@@ -13458,15 +13894,40 @@
         <v>-946</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1468</v>
       </c>
       <c r="L18" s="4">
         <f>SUM(K$4:K18)</f>
         <v>16943</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <v>66</v>
+      </c>
+      <c r="Q18">
+        <v>154</v>
+      </c>
+      <c r="R18">
+        <v>-600</v>
+      </c>
+      <c r="S18">
+        <v>-110</v>
+      </c>
+      <c r="T18">
+        <v>-600</v>
+      </c>
+      <c r="U18">
+        <v>410</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="3"/>
+        <v>-680</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>-934</v>
       </c>
@@ -13486,15 +13947,40 @@
         <v>538</v>
       </c>
       <c r="K19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-491.66666666666669</v>
       </c>
       <c r="L19" s="4">
         <f>SUM(K$4:K19)</f>
         <v>16451.333333333332</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>-800</v>
+      </c>
+      <c r="Q19">
+        <v>-490</v>
+      </c>
+      <c r="R19">
+        <v>19617</v>
+      </c>
+      <c r="S19">
+        <v>-300</v>
+      </c>
+      <c r="T19">
+        <v>15969</v>
+      </c>
+      <c r="U19">
+        <v>-536</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="3"/>
+        <v>33460</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>-879</v>
       </c>
@@ -13514,15 +14000,40 @@
         <v>27389</v>
       </c>
       <c r="K20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19715.333333333332</v>
       </c>
       <c r="L20" s="4">
         <f>SUM(K$4:K20)</f>
         <v>36166.666666666664</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <v>-471</v>
+      </c>
+      <c r="Q20">
+        <v>301</v>
+      </c>
+      <c r="R20">
+        <v>-700</v>
+      </c>
+      <c r="S20">
+        <v>-700</v>
+      </c>
+      <c r="T20">
+        <v>-700</v>
+      </c>
+      <c r="U20">
+        <v>-700</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="3"/>
+        <v>-2970</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>-1273</v>
       </c>
@@ -13542,15 +14053,40 @@
         <v>-828</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2292.6666666666665</v>
       </c>
       <c r="L21" s="4">
         <f>SUM(K$4:K21)</f>
         <v>33874</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <v>2202</v>
+      </c>
+      <c r="Q21">
+        <v>-112</v>
+      </c>
+      <c r="R21">
+        <v>4239</v>
+      </c>
+      <c r="S21">
+        <v>1770</v>
+      </c>
+      <c r="T21">
+        <v>4663</v>
+      </c>
+      <c r="U21">
+        <v>-600</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="3"/>
+        <v>12162</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>2161</v>
       </c>
@@ -13570,15 +14106,40 @@
         <v>-802</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7475.666666666667</v>
       </c>
       <c r="L22" s="4">
         <f>SUM(K$4:K22)</f>
         <v>41349.666666666664</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <v>1559</v>
+      </c>
+      <c r="Q22">
+        <v>1208</v>
+      </c>
+      <c r="R22">
+        <v>-600</v>
+      </c>
+      <c r="S22">
+        <v>190</v>
+      </c>
+      <c r="T22">
+        <v>-600</v>
+      </c>
+      <c r="U22">
+        <v>-110</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="3"/>
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>1092</v>
       </c>
@@ -13598,15 +14159,40 @@
         <v>1691</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>477.66666666666669</v>
       </c>
       <c r="L23" s="4">
         <f>SUM(K$4:K23)</f>
         <v>41827.333333333328</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <v>-600</v>
+      </c>
+      <c r="Q23">
+        <v>-24</v>
+      </c>
+      <c r="R23">
+        <v>-600</v>
+      </c>
+      <c r="S23">
+        <v>-270</v>
+      </c>
+      <c r="T23">
+        <v>-600</v>
+      </c>
+      <c r="U23">
+        <v>-348</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="3"/>
+        <v>-2442</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>-829</v>
       </c>
@@ -13626,15 +14212,40 @@
         <v>-942</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1934</v>
       </c>
       <c r="L24" s="4">
         <f>SUM(K$4:K24)</f>
         <v>39893.333333333328</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <v>-600</v>
+      </c>
+      <c r="Q24">
+        <v>-152</v>
+      </c>
+      <c r="R24">
+        <v>-600</v>
+      </c>
+      <c r="S24">
+        <v>-430</v>
+      </c>
+      <c r="T24">
+        <v>-600</v>
+      </c>
+      <c r="U24">
+        <v>32</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="3"/>
+        <v>-2350</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>1463</v>
       </c>
@@ -13654,15 +14265,40 @@
         <v>-542</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100.66666666666667</v>
       </c>
       <c r="L25" s="4">
         <f>SUM(K$4:K25)</f>
         <v>39993.999999999993</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <v>-600</v>
+      </c>
+      <c r="Q25">
+        <v>247</v>
+      </c>
+      <c r="R25">
+        <v>-600</v>
+      </c>
+      <c r="S25">
+        <v>10</v>
+      </c>
+      <c r="T25">
+        <v>-600</v>
+      </c>
+      <c r="U25">
+        <v>2162</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="3"/>
+        <v>619</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>-559</v>
       </c>
@@ -13682,15 +14318,40 @@
         <v>1282</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-950.66666666666663</v>
       </c>
       <c r="L26" s="4">
         <f>SUM(K$4:K26)</f>
         <v>39043.333333333328</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <v>4136</v>
+      </c>
+      <c r="Q26">
+        <v>-350</v>
+      </c>
+      <c r="R26">
+        <v>-600</v>
+      </c>
+      <c r="S26">
+        <v>-600</v>
+      </c>
+      <c r="T26">
+        <v>-600</v>
+      </c>
+      <c r="U26">
+        <v>-600</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="3"/>
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>3401</v>
       </c>
@@ -13710,15 +14371,40 @@
         <v>514</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>500.66666666666669</v>
       </c>
       <c r="L27" s="4">
         <f>SUM(K$4:K27)</f>
         <v>39543.999999999993</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <v>161</v>
+      </c>
+      <c r="Q27">
+        <v>922</v>
+      </c>
+      <c r="R27">
+        <v>-310</v>
+      </c>
+      <c r="S27">
+        <v>1470</v>
+      </c>
+      <c r="T27">
+        <v>-330</v>
+      </c>
+      <c r="U27">
+        <v>2839</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="3"/>
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>938</v>
       </c>
@@ -13738,15 +14424,40 @@
         <v>2123</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2487.6666666666665</v>
       </c>
       <c r="L28" s="4">
         <f>SUM(K$4:K28)</f>
         <v>42031.666666666657</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <v>-342</v>
+      </c>
+      <c r="Q28">
+        <v>8</v>
+      </c>
+      <c r="R28">
+        <v>-600</v>
+      </c>
+      <c r="S28">
+        <v>-460</v>
+      </c>
+      <c r="T28">
+        <v>-600</v>
+      </c>
+      <c r="U28">
+        <v>828</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="3"/>
+        <v>-1166</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>904</v>
       </c>
@@ -13766,15 +14477,40 @@
         <v>716</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3679.3333333333335</v>
       </c>
       <c r="L29" s="4">
         <f>SUM(K$4:K29)</f>
         <v>45710.999999999993</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P29">
+        <v>-231</v>
+      </c>
+      <c r="Q29">
+        <v>-380</v>
+      </c>
+      <c r="R29">
+        <v>-600</v>
+      </c>
+      <c r="S29">
+        <v>-600</v>
+      </c>
+      <c r="T29">
+        <v>-600</v>
+      </c>
+      <c r="U29">
+        <v>-600</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="3"/>
+        <v>-3011</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>1092</v>
       </c>
@@ -13794,15 +14530,40 @@
         <v>-1160</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1537</v>
       </c>
       <c r="L30" s="4">
         <f>SUM(K$4:K30)</f>
         <v>44173.999999999993</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P30">
+        <v>-600</v>
+      </c>
+      <c r="Q30">
+        <v>-260</v>
+      </c>
+      <c r="R30">
+        <v>-600</v>
+      </c>
+      <c r="S30">
+        <v>-600</v>
+      </c>
+      <c r="T30">
+        <v>-600</v>
+      </c>
+      <c r="U30">
+        <v>-404</v>
+      </c>
+      <c r="V30">
+        <v>3060</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="3"/>
+        <v>-3064</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>2963</v>
       </c>
@@ -13822,15 +14583,40 @@
         <v>796</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-348.33333333333331</v>
       </c>
       <c r="L31" s="4">
         <f>SUM(K$4:K31)</f>
         <v>43825.666666666657</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <v>27</v>
+      </c>
+      <c r="Q31">
+        <v>320</v>
+      </c>
+      <c r="R31">
+        <v>-600</v>
+      </c>
+      <c r="S31">
+        <v>2748</v>
+      </c>
+      <c r="T31">
+        <v>-600</v>
+      </c>
+      <c r="U31">
+        <v>2466</v>
+      </c>
+      <c r="V31">
+        <v>-576</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="3"/>
+        <v>4361</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>743</v>
       </c>
@@ -13850,15 +14636,40 @@
         <v>2166</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1026.6666666666667</v>
       </c>
       <c r="L32" s="4">
         <f>SUM(K$4:K32)</f>
         <v>44852.333333333321</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P32">
+        <v>-600</v>
+      </c>
+      <c r="Q32">
+        <v>-281</v>
+      </c>
+      <c r="R32">
+        <v>-600</v>
+      </c>
+      <c r="S32">
+        <v>-250</v>
+      </c>
+      <c r="T32">
+        <v>-600</v>
+      </c>
+      <c r="U32">
+        <v>-182</v>
+      </c>
+      <c r="V32">
+        <v>-576</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="3"/>
+        <v>-2513</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>-534</v>
       </c>
@@ -13878,15 +14689,40 @@
         <v>-1182</v>
       </c>
       <c r="K33" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1830.6666666666667</v>
       </c>
       <c r="L33" s="4">
         <f>SUM(K$4:K33)</f>
         <v>43021.666666666657</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P33">
+        <v>1710</v>
+      </c>
+      <c r="Q33">
+        <v>-71</v>
+      </c>
+      <c r="R33">
+        <v>1500</v>
+      </c>
+      <c r="S33">
+        <v>1820</v>
+      </c>
+      <c r="T33">
+        <v>1193</v>
+      </c>
+      <c r="U33">
+        <v>280</v>
+      </c>
+      <c r="V33">
+        <v>726</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="3"/>
+        <v>6432</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>2693</v>
       </c>
@@ -13906,15 +14742,40 @@
         <v>-366</v>
       </c>
       <c r="K34" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15840</v>
       </c>
       <c r="L34" s="4">
         <f>SUM(K$4:K34)</f>
         <v>58861.666666666657</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P34">
+        <v>-600</v>
+      </c>
+      <c r="Q34">
+        <v>-112</v>
+      </c>
+      <c r="R34">
+        <v>1910</v>
+      </c>
+      <c r="S34">
+        <v>230</v>
+      </c>
+      <c r="T34">
+        <v>2337</v>
+      </c>
+      <c r="U34">
+        <v>914</v>
+      </c>
+      <c r="V34">
+        <v>-576</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="3"/>
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>-573</v>
       </c>
@@ -13934,15 +14795,40 @@
         <v>144</v>
       </c>
       <c r="K35" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>490.66666666666669</v>
       </c>
       <c r="L35" s="4">
         <f>SUM(K$4:K35)</f>
         <v>59352.333333333321</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <v>-600</v>
+      </c>
+      <c r="Q35">
+        <v>86</v>
+      </c>
+      <c r="R35">
+        <v>-600</v>
+      </c>
+      <c r="S35">
+        <v>-600</v>
+      </c>
+      <c r="T35">
+        <v>-600</v>
+      </c>
+      <c r="U35">
+        <v>-600</v>
+      </c>
+      <c r="V35">
+        <v>-211</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="3"/>
+        <v>-2914</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>-337</v>
       </c>
@@ -13962,15 +14848,40 @@
         <v>-1458</v>
       </c>
       <c r="K36" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2113.6666666666665</v>
       </c>
       <c r="L36" s="4">
         <f>SUM(K$4:K36)</f>
         <v>57238.666666666657</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P36">
+        <v>4689</v>
+      </c>
+      <c r="Q36">
+        <v>-261</v>
+      </c>
+      <c r="R36">
+        <v>179</v>
+      </c>
+      <c r="S36">
+        <v>-90</v>
+      </c>
+      <c r="T36">
+        <v>67</v>
+      </c>
+      <c r="U36">
+        <v>-298</v>
+      </c>
+      <c r="V36">
+        <v>-1440</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="3"/>
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>10156</v>
       </c>
@@ -13990,15 +14901,40 @@
         <v>28</v>
       </c>
       <c r="K37" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2504.3333333333335</v>
       </c>
       <c r="L37" s="4">
         <f>SUM(K$4:K37)</f>
         <v>59742.999999999993</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P37">
+        <v>2598</v>
+      </c>
+      <c r="Q37">
+        <v>-522</v>
+      </c>
+      <c r="R37">
+        <v>-1500</v>
+      </c>
+      <c r="S37">
+        <v>-940</v>
+      </c>
+      <c r="T37">
+        <v>-1500</v>
+      </c>
+      <c r="U37">
+        <v>-20</v>
+      </c>
+      <c r="V37">
+        <v>-384</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="3"/>
+        <v>-1884</v>
+      </c>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>2598</v>
       </c>
@@ -14018,15 +14954,40 @@
         <v>-20</v>
       </c>
       <c r="K38" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-628</v>
       </c>
       <c r="L38" s="4">
         <f>SUM(K$4:K38)</f>
         <v>59114.999999999993</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <v>-400</v>
+      </c>
+      <c r="Q38">
+        <v>78</v>
+      </c>
+      <c r="R38">
+        <v>149</v>
+      </c>
+      <c r="S38">
+        <v>170</v>
+      </c>
+      <c r="T38">
+        <v>163</v>
+      </c>
+      <c r="U38">
+        <v>-356</v>
+      </c>
+      <c r="V38">
+        <v>-480</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="3"/>
+        <v>-196</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>3435</v>
       </c>
@@ -14046,15 +15007,40 @@
         <v>-1398</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-265</v>
       </c>
       <c r="L39" s="4">
         <f>SUM(K$4:K39)</f>
         <v>58849.999999999993</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <v>-700</v>
+      </c>
+      <c r="Q39">
+        <v>-52</v>
+      </c>
+      <c r="R39">
+        <v>-700</v>
+      </c>
+      <c r="S39">
+        <v>-480</v>
+      </c>
+      <c r="T39">
+        <v>-700</v>
+      </c>
+      <c r="U39">
+        <v>-600</v>
+      </c>
+      <c r="V39">
+        <v>-576</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="3"/>
+        <v>-3232</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>454</v>
       </c>
@@ -14074,15 +15060,40 @@
         <v>-1426</v>
       </c>
       <c r="K40" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2149</v>
       </c>
       <c r="L40" s="4">
         <f>SUM(K$4:K40)</f>
         <v>56700.999999999993</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <v>1709</v>
+      </c>
+      <c r="Q40">
+        <v>-222</v>
+      </c>
+      <c r="R40">
+        <v>-600</v>
+      </c>
+      <c r="S40">
+        <v>600</v>
+      </c>
+      <c r="T40">
+        <v>-600</v>
+      </c>
+      <c r="U40">
+        <v>114</v>
+      </c>
+      <c r="V40">
+        <v>-576</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="3"/>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>1781</v>
       </c>
@@ -14102,15 +15113,40 @@
         <v>528</v>
       </c>
       <c r="K41" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>170.66666666666666</v>
       </c>
       <c r="L41" s="4">
         <f>SUM(K$4:K41)</f>
         <v>56871.666666666657</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P41">
+        <v>1519</v>
+      </c>
+      <c r="Q41">
+        <v>-43</v>
+      </c>
+      <c r="R41">
+        <v>-600</v>
+      </c>
+      <c r="S41">
+        <v>-30</v>
+      </c>
+      <c r="T41">
+        <v>-600</v>
+      </c>
+      <c r="U41">
+        <v>-246</v>
+      </c>
+      <c r="V41">
+        <v>-264</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>1819</v>
       </c>
@@ -14130,15 +15166,40 @@
         <v>-562</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>817.33333333333337</v>
       </c>
       <c r="L42" s="4">
         <f>SUM(K$4:K42)</f>
         <v>57688.999999999993</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P42">
+        <v>-331</v>
+      </c>
+      <c r="Q42">
+        <v>-240</v>
+      </c>
+      <c r="R42">
+        <v>-500</v>
+      </c>
+      <c r="S42">
+        <v>-300</v>
+      </c>
+      <c r="T42">
+        <v>-500</v>
+      </c>
+      <c r="U42">
+        <v>-416</v>
+      </c>
+      <c r="V42">
+        <v>-480</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="3"/>
+        <v>-2287</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>2637</v>
       </c>
@@ -14158,15 +15219,40 @@
         <v>-1190</v>
       </c>
       <c r="K43" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-302</v>
       </c>
       <c r="L43" s="4">
         <f>SUM(K$4:K43)</f>
         <v>57386.999999999993</v>
       </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P43">
+        <v>-700</v>
+      </c>
+      <c r="Q43">
+        <v>284</v>
+      </c>
+      <c r="R43">
+        <v>128</v>
+      </c>
+      <c r="S43">
+        <v>600</v>
+      </c>
+      <c r="T43">
+        <v>-73</v>
+      </c>
+      <c r="U43">
+        <v>352</v>
+      </c>
+      <c r="V43">
+        <v>-576</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="3"/>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>-1290</v>
       </c>
@@ -14186,15 +15272,40 @@
         <v>-748</v>
       </c>
       <c r="K44" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1212.3333333333333</v>
       </c>
       <c r="L44" s="4">
         <f>SUM(K$4:K44)</f>
         <v>58599.333333333328</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P44">
+        <v>-600</v>
+      </c>
+      <c r="Q44">
+        <v>245</v>
+      </c>
+      <c r="R44">
+        <v>2486</v>
+      </c>
+      <c r="S44">
+        <v>1550</v>
+      </c>
+      <c r="T44">
+        <v>2661</v>
+      </c>
+      <c r="U44">
+        <v>1430</v>
+      </c>
+      <c r="V44">
+        <v>-576</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="3"/>
+        <v>7772</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>1283</v>
       </c>
@@ -14214,15 +15325,40 @@
         <v>430</v>
       </c>
       <c r="K45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2133.6666666666665</v>
       </c>
       <c r="L45" s="4">
         <f>SUM(K$4:K45)</f>
         <v>60732.999999999993</v>
       </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P45">
+        <v>-600</v>
+      </c>
+      <c r="Q45">
+        <v>215</v>
+      </c>
+      <c r="R45">
+        <v>-600</v>
+      </c>
+      <c r="S45">
+        <v>-480</v>
+      </c>
+      <c r="T45">
+        <v>-600</v>
+      </c>
+      <c r="U45">
+        <v>-562</v>
+      </c>
+      <c r="V45">
+        <v>7156</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="3"/>
+        <v>-2627</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>-1057</v>
       </c>
@@ -14242,15 +15378,40 @@
         <v>-1562</v>
       </c>
       <c r="K46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2134</v>
       </c>
       <c r="L46" s="4">
         <f>SUM(K$4:K46)</f>
         <v>58598.999999999993</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P46">
+        <v>-600</v>
+      </c>
+      <c r="Q46">
+        <v>-92</v>
+      </c>
+      <c r="R46">
+        <v>149</v>
+      </c>
+      <c r="S46">
+        <v>650</v>
+      </c>
+      <c r="T46">
+        <v>142</v>
+      </c>
+      <c r="U46">
+        <v>-336</v>
+      </c>
+      <c r="V46">
+        <v>7037</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="3"/>
+        <v>-87</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>-618</v>
       </c>
@@ -14270,15 +15431,40 @@
         <v>1630</v>
       </c>
       <c r="K47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1322.6666666666667</v>
       </c>
       <c r="L47" s="4">
         <f>SUM(K$4:K47)</f>
         <v>59921.666666666657</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P47">
+        <v>1392</v>
+      </c>
+      <c r="Q47">
+        <v>38</v>
+      </c>
+      <c r="R47">
+        <v>-600</v>
+      </c>
+      <c r="S47">
+        <v>330</v>
+      </c>
+      <c r="T47">
+        <v>-600</v>
+      </c>
+      <c r="U47">
+        <v>-148</v>
+      </c>
+      <c r="V47">
+        <v>-576</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="3"/>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>1015</v>
       </c>
@@ -14298,15 +15484,40 @@
         <v>-688</v>
       </c>
       <c r="K48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-702.66666666666663</v>
       </c>
       <c r="L48" s="4">
         <f>SUM(K$4:K48)</f>
         <v>59218.999999999993</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P48">
+        <v>-146</v>
+      </c>
+      <c r="Q48">
+        <v>-191</v>
+      </c>
+      <c r="R48">
+        <v>-600</v>
+      </c>
+      <c r="S48">
+        <v>-600</v>
+      </c>
+      <c r="T48">
+        <v>-600</v>
+      </c>
+      <c r="U48">
+        <v>-600</v>
+      </c>
+      <c r="V48">
+        <v>-576</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="3"/>
+        <v>-2737</v>
+      </c>
+    </row>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>3437</v>
       </c>
@@ -14326,15 +15537,40 @@
         <v>2498</v>
       </c>
       <c r="K49" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1547.6666666666667</v>
       </c>
       <c r="L49" s="4">
         <f>SUM(K$4:K49)</f>
         <v>60766.666666666657</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P49">
+        <v>-39</v>
+      </c>
+      <c r="Q49">
+        <v>68</v>
+      </c>
+      <c r="R49">
+        <v>-600</v>
+      </c>
+      <c r="S49">
+        <v>-180</v>
+      </c>
+      <c r="T49">
+        <v>-600</v>
+      </c>
+      <c r="U49">
+        <v>2361</v>
+      </c>
+      <c r="V49">
+        <v>-576</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>-757</v>
       </c>
@@ -14354,15 +15590,40 @@
         <v>2137</v>
       </c>
       <c r="K50" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2852.6666666666665</v>
       </c>
       <c r="L50" s="4">
         <f>SUM(K$4:K50)</f>
         <v>63619.333333333321</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P50">
+        <v>1004</v>
+      </c>
+      <c r="Q50">
+        <v>-171</v>
+      </c>
+      <c r="R50">
+        <v>773</v>
+      </c>
+      <c r="S50">
+        <v>350</v>
+      </c>
+      <c r="T50">
+        <v>931</v>
+      </c>
+      <c r="U50">
+        <v>-130</v>
+      </c>
+      <c r="V50">
+        <v>-218</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="3"/>
+        <v>2757</v>
+      </c>
+    </row>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>1736</v>
       </c>
@@ -14382,15 +15643,40 @@
         <v>1398</v>
       </c>
       <c r="K51" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1814.6666666666667</v>
       </c>
       <c r="L51" s="4">
         <f>SUM(K$4:K51)</f>
         <v>65433.999999999985</v>
       </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P51">
+        <v>1429</v>
+      </c>
+      <c r="Q51">
+        <v>-360</v>
+      </c>
+      <c r="R51">
+        <v>-600</v>
+      </c>
+      <c r="S51">
+        <v>-450</v>
+      </c>
+      <c r="T51">
+        <v>-600</v>
+      </c>
+      <c r="U51">
+        <v>7782</v>
+      </c>
+      <c r="V51">
+        <v>-223</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="3"/>
+        <v>7201</v>
+      </c>
+    </row>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>0</v>
       </c>
@@ -14410,7 +15696,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L52" s="4">
@@ -14426,1023 +15712,552 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:J51"/>
+  <dimension ref="D2:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E2">
-        <f>SUM(E3:E101)</f>
-        <v>41152</v>
+    <row r="2" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1234</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:J2" si="0">SUM(F3:F101)</f>
-        <v>34963</v>
-      </c>
-      <c r="G2">
+        <v>12345</v>
+      </c>
+      <c r="G2" s="5">
+        <v>234</v>
+      </c>
+      <c r="H2">
+        <v>2345</v>
+      </c>
+      <c r="I2">
+        <v>234</v>
+      </c>
+      <c r="J2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f>SUM(D4:D27)</f>
+        <v>-1895</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:J3" si="0">SUM(E4:E27)</f>
+        <v>3184</v>
+      </c>
+      <c r="F3">
         <f t="shared" si="0"/>
-        <v>19736</v>
-      </c>
-      <c r="H2">
+        <v>987</v>
+      </c>
+      <c r="G3" s="5">
         <f t="shared" si="0"/>
-        <v>238</v>
-      </c>
-      <c r="I2">
+        <v>8742</v>
+      </c>
+      <c r="H3">
         <f t="shared" si="0"/>
-        <v>-16034</v>
-      </c>
-      <c r="J2">
+        <v>-6550</v>
+      </c>
+      <c r="I3">
         <f t="shared" si="0"/>
-        <v>-14870</v>
-      </c>
-    </row>
-    <row r="3" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E3">
-        <v>-434</v>
-      </c>
-      <c r="F3">
-        <v>-619</v>
-      </c>
-      <c r="G3">
-        <v>-1420</v>
-      </c>
-      <c r="H3">
-        <v>890</v>
-      </c>
-      <c r="I3">
-        <v>160</v>
+        <v>8742</v>
       </c>
       <c r="J3">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="4" spans="5:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-10886</v>
+      </c>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>-576</v>
+      </c>
       <c r="E4">
-        <v>4682</v>
+        <v>3850</v>
       </c>
       <c r="F4">
-        <v>3474</v>
+        <v>952</v>
       </c>
       <c r="G4">
-        <v>-180</v>
+        <v>3060</v>
       </c>
       <c r="H4">
-        <v>-1700</v>
+        <v>559</v>
       </c>
       <c r="I4">
-        <v>-840</v>
+        <v>3060</v>
       </c>
       <c r="J4">
-        <v>-770</v>
-      </c>
-    </row>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>-576</v>
+      </c>
       <c r="E5">
-        <v>871</v>
+        <v>-323</v>
       </c>
       <c r="F5">
-        <v>425</v>
+        <v>-297</v>
       </c>
       <c r="G5">
-        <v>-40</v>
+        <v>-576</v>
       </c>
       <c r="H5">
-        <v>-750</v>
+        <v>-576</v>
       </c>
       <c r="I5">
-        <v>-910</v>
+        <v>-576</v>
       </c>
       <c r="J5">
-        <v>-1450</v>
-      </c>
-    </row>
-    <row r="6" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>4492</v>
+      </c>
       <c r="E6">
-        <v>-1274</v>
+        <v>1113</v>
       </c>
       <c r="F6">
-        <v>-1291</v>
+        <v>135</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>-576</v>
       </c>
       <c r="H6">
-        <v>-760</v>
+        <v>-576</v>
       </c>
       <c r="I6">
-        <v>-490</v>
+        <v>-576</v>
       </c>
       <c r="J6">
-        <v>-130</v>
-      </c>
-    </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>-576</v>
+      </c>
       <c r="E7">
-        <v>100</v>
+        <v>-250</v>
       </c>
       <c r="F7">
-        <v>-272</v>
+        <v>319</v>
       </c>
       <c r="G7">
-        <v>-80</v>
+        <v>726</v>
       </c>
       <c r="H7">
-        <v>5254</v>
+        <v>-83</v>
       </c>
       <c r="I7">
-        <v>860</v>
+        <v>726</v>
       </c>
       <c r="J7">
-        <v>-1870</v>
-      </c>
-    </row>
-    <row r="8" spans="5:10" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>-576</v>
+      </c>
       <c r="E8">
-        <v>-600</v>
+        <v>-576</v>
       </c>
       <c r="F8">
-        <v>144</v>
+        <v>-360</v>
       </c>
       <c r="G8">
-        <v>-600</v>
+        <v>-576</v>
       </c>
       <c r="H8">
-        <v>1880</v>
+        <v>-576</v>
       </c>
       <c r="I8">
-        <v>-600</v>
+        <v>-576</v>
       </c>
       <c r="J8">
-        <v>-600</v>
-      </c>
-    </row>
-    <row r="9" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>-576</v>
+      </c>
       <c r="E9">
-        <v>1606</v>
+        <v>-271</v>
       </c>
       <c r="F9">
-        <v>1082</v>
+        <v>-284</v>
       </c>
       <c r="G9">
-        <v>2756</v>
+        <v>-211</v>
       </c>
       <c r="H9">
-        <v>-870</v>
+        <v>-485</v>
       </c>
       <c r="I9">
-        <v>-940</v>
+        <v>-211</v>
       </c>
       <c r="J9">
-        <v>-1500</v>
-      </c>
-    </row>
-    <row r="10" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>216</v>
+      </c>
       <c r="E10">
-        <v>-1200</v>
+        <v>47</v>
       </c>
       <c r="F10">
-        <v>-1216</v>
+        <v>-376</v>
       </c>
       <c r="G10">
-        <v>1580</v>
+        <v>-1440</v>
       </c>
       <c r="H10">
-        <v>-1090</v>
+        <v>-1209</v>
       </c>
       <c r="I10">
-        <v>-1300</v>
+        <v>-1440</v>
       </c>
       <c r="J10">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="11" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-515</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>-384</v>
+      </c>
       <c r="E11">
-        <v>1394</v>
+        <v>-360</v>
       </c>
       <c r="F11">
-        <v>1250</v>
+        <v>-234</v>
       </c>
       <c r="G11">
-        <v>-730</v>
+        <v>-384</v>
       </c>
       <c r="H11">
-        <v>690</v>
+        <v>-384</v>
       </c>
       <c r="I11">
-        <v>-1600</v>
+        <v>-384</v>
       </c>
       <c r="J11">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-384</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>-242</v>
+      </c>
       <c r="E12">
-        <v>882</v>
+        <v>-420</v>
       </c>
       <c r="F12">
-        <v>488</v>
+        <v>-285</v>
       </c>
       <c r="G12">
-        <v>2328</v>
+        <v>-480</v>
       </c>
       <c r="H12">
-        <v>-1400</v>
+        <v>-480</v>
       </c>
       <c r="I12">
-        <v>-1090</v>
+        <v>-480</v>
       </c>
       <c r="J12">
-        <v>-1030</v>
-      </c>
-    </row>
-    <row r="13" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-480</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>3047</v>
+      </c>
       <c r="E13">
-        <v>-1520</v>
+        <v>555</v>
       </c>
       <c r="F13">
+        <v>165</v>
+      </c>
+      <c r="G13">
+        <v>-576</v>
+      </c>
+      <c r="H13">
+        <v>-576</v>
+      </c>
+      <c r="I13">
+        <v>-576</v>
+      </c>
+      <c r="J13">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>-576</v>
+      </c>
+      <c r="E14">
+        <v>-414</v>
+      </c>
+      <c r="F14">
+        <v>-319</v>
+      </c>
+      <c r="G14">
+        <v>-576</v>
+      </c>
+      <c r="H14">
+        <v>-576</v>
+      </c>
+      <c r="I14">
+        <v>-576</v>
+      </c>
+      <c r="J14">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>-480</v>
+      </c>
+      <c r="E15">
+        <v>-352</v>
+      </c>
+      <c r="F15">
+        <v>-268</v>
+      </c>
+      <c r="G15">
+        <v>-264</v>
+      </c>
+      <c r="H15">
+        <v>-426</v>
+      </c>
+      <c r="I15">
+        <v>-264</v>
+      </c>
+      <c r="J15">
+        <v>-480</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>-480</v>
+      </c>
+      <c r="E16">
+        <v>-367</v>
+      </c>
+      <c r="F16">
+        <v>-203</v>
+      </c>
+      <c r="G16">
+        <v>-480</v>
+      </c>
+      <c r="H16">
+        <v>-480</v>
+      </c>
+      <c r="I16">
+        <v>-480</v>
+      </c>
+      <c r="J16">
+        <v>-480</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>-576</v>
+      </c>
+      <c r="E17">
         <v>-318</v>
       </c>
-      <c r="G13">
-        <v>-1210</v>
-      </c>
-      <c r="H13">
-        <v>880</v>
-      </c>
-      <c r="I13">
-        <v>-820</v>
-      </c>
-      <c r="J13">
-        <v>-1450</v>
-      </c>
-    </row>
-    <row r="14" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E14">
-        <v>8021</v>
-      </c>
-      <c r="F14">
-        <v>7116</v>
-      </c>
-      <c r="G14">
-        <v>7546</v>
-      </c>
-      <c r="H14">
-        <v>1400</v>
-      </c>
-      <c r="I14">
-        <v>-700</v>
-      </c>
-      <c r="J14">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="15" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E15">
-        <v>-1406</v>
-      </c>
-      <c r="F15">
-        <v>-1381</v>
-      </c>
-      <c r="G15">
-        <v>1300</v>
-      </c>
-      <c r="H15">
-        <v>-1600</v>
-      </c>
-      <c r="I15">
-        <v>450</v>
-      </c>
-      <c r="J15">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="16" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E16">
-        <v>-158</v>
-      </c>
-      <c r="F16">
-        <v>-304</v>
-      </c>
-      <c r="G16">
-        <v>310</v>
-      </c>
-      <c r="H16">
-        <v>-1450</v>
-      </c>
-      <c r="I16">
-        <v>1540</v>
-      </c>
-      <c r="J16">
-        <v>-1070</v>
-      </c>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E17">
-        <v>-946</v>
-      </c>
       <c r="F17">
-        <v>-869</v>
+        <v>280</v>
       </c>
       <c r="G17">
-        <v>2782</v>
+        <v>-576</v>
       </c>
       <c r="H17">
-        <v>-880</v>
+        <v>-576</v>
       </c>
       <c r="I17">
-        <v>-1600</v>
+        <v>-576</v>
       </c>
       <c r="J17">
-        <v>1390</v>
-      </c>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>-576</v>
+      </c>
       <c r="E18">
-        <v>538</v>
+        <v>-576</v>
       </c>
       <c r="F18">
-        <v>174</v>
+        <v>-356</v>
       </c>
       <c r="G18">
-        <v>4768</v>
+        <v>-576</v>
       </c>
       <c r="H18">
-        <v>310</v>
+        <v>-576</v>
       </c>
       <c r="I18">
-        <v>-720</v>
+        <v>-576</v>
       </c>
       <c r="J18">
-        <v>3532</v>
-      </c>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>-576</v>
+      </c>
       <c r="E19">
-        <v>27389</v>
+        <v>1612</v>
       </c>
       <c r="F19">
-        <v>21656</v>
+        <v>308</v>
       </c>
       <c r="G19">
-        <v>-830</v>
+        <v>7156</v>
       </c>
       <c r="H19">
-        <v>-700</v>
+        <v>1357</v>
       </c>
       <c r="I19">
-        <v>1786</v>
+        <v>7156</v>
       </c>
       <c r="J19">
-        <v>-330</v>
-      </c>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>-576</v>
+      </c>
       <c r="E20">
-        <v>-828</v>
+        <v>1987</v>
       </c>
       <c r="F20">
-        <v>-874</v>
+        <v>399</v>
       </c>
       <c r="G20">
-        <v>3468</v>
+        <v>7037</v>
       </c>
       <c r="H20">
-        <v>-200</v>
+        <v>1327</v>
       </c>
       <c r="I20">
-        <v>-1700</v>
+        <v>7037</v>
       </c>
       <c r="J20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>-576</v>
+      </c>
       <c r="E21">
-        <v>-802</v>
+        <v>-576</v>
       </c>
       <c r="F21">
-        <v>-696</v>
+        <v>-360</v>
       </c>
       <c r="G21">
-        <v>-1600</v>
+        <v>-576</v>
       </c>
       <c r="H21">
-        <v>-1070</v>
+        <v>-576</v>
       </c>
       <c r="I21">
-        <v>-1050</v>
+        <v>-576</v>
       </c>
       <c r="J21">
-        <v>-1090</v>
-      </c>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>-576</v>
+      </c>
       <c r="E22">
-        <v>1691</v>
+        <v>-378</v>
       </c>
       <c r="F22">
-        <v>1458</v>
+        <v>669</v>
       </c>
       <c r="G22">
-        <v>-980</v>
+        <v>-576</v>
       </c>
       <c r="H22">
-        <v>1280</v>
+        <v>-576</v>
       </c>
       <c r="I22">
-        <v>-740</v>
+        <v>-576</v>
       </c>
       <c r="J22">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>-576</v>
+      </c>
       <c r="E23">
-        <v>-942</v>
+        <v>-576</v>
       </c>
       <c r="F23">
-        <v>-946</v>
+        <v>-196</v>
       </c>
       <c r="G23">
-        <v>1878</v>
+        <v>-576</v>
       </c>
       <c r="H23">
-        <v>-910</v>
+        <v>-576</v>
       </c>
       <c r="I23">
-        <v>-1410</v>
+        <v>-576</v>
       </c>
       <c r="J23">
-        <v>-370</v>
-      </c>
-    </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.3">
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>-576</v>
+      </c>
       <c r="E24">
-        <v>-542</v>
+        <v>-223</v>
       </c>
       <c r="F24">
-        <v>-690</v>
+        <v>1298</v>
       </c>
       <c r="G24">
-        <v>-1100</v>
+        <v>-218</v>
       </c>
       <c r="H24">
-        <v>940</v>
+        <v>-486</v>
       </c>
       <c r="I24">
-        <v>-210</v>
+        <v>-218</v>
       </c>
       <c r="J24">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E25">
-        <v>1282</v>
-      </c>
-      <c r="F25">
-        <v>878</v>
-      </c>
-      <c r="G25">
-        <v>600</v>
-      </c>
-      <c r="H25">
-        <v>-1180</v>
-      </c>
-      <c r="I25">
-        <v>-630</v>
-      </c>
-      <c r="J25">
-        <v>-760</v>
-      </c>
-    </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E26">
-        <v>514</v>
-      </c>
-      <c r="F26">
-        <v>206</v>
-      </c>
-      <c r="G26">
-        <v>1242</v>
-      </c>
-      <c r="H26">
-        <v>1054</v>
-      </c>
-      <c r="I26">
-        <v>-1220</v>
-      </c>
-      <c r="J26">
-        <v>-1290</v>
-      </c>
-    </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E27">
-        <v>2123</v>
-      </c>
-      <c r="F27">
-        <v>1518</v>
-      </c>
-      <c r="G27">
-        <v>220</v>
-      </c>
-      <c r="H27">
-        <v>-160</v>
-      </c>
-      <c r="I27">
-        <v>-50</v>
-      </c>
-      <c r="J27">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E28">
-        <v>716</v>
-      </c>
-      <c r="F28">
-        <v>1061</v>
-      </c>
-      <c r="G28">
-        <v>480</v>
-      </c>
-      <c r="H28">
-        <v>550</v>
-      </c>
-      <c r="I28">
-        <v>-1120</v>
-      </c>
-      <c r="J28">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E29">
-        <v>-1160</v>
-      </c>
-      <c r="F29">
-        <v>-1184</v>
-      </c>
-      <c r="G29">
-        <v>-1410</v>
-      </c>
-      <c r="H29">
-        <v>-1430</v>
-      </c>
-      <c r="I29">
-        <v>-550</v>
-      </c>
-      <c r="J29">
-        <v>-380</v>
-      </c>
-    </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E30">
-        <v>796</v>
-      </c>
-      <c r="F30">
-        <v>733</v>
-      </c>
-      <c r="G30">
-        <v>-1470</v>
-      </c>
-      <c r="H30">
-        <v>1944</v>
-      </c>
-      <c r="I30">
-        <v>7982</v>
-      </c>
-      <c r="J30">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E31">
-        <v>2166</v>
-      </c>
-      <c r="F31">
-        <v>1644</v>
-      </c>
-      <c r="G31">
-        <v>960</v>
-      </c>
-      <c r="H31">
-        <v>130</v>
-      </c>
-      <c r="I31">
-        <v>-260</v>
-      </c>
-      <c r="J31">
-        <v>-850</v>
-      </c>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E32">
-        <v>-1182</v>
-      </c>
-      <c r="F32">
-        <v>-1136</v>
-      </c>
-      <c r="G32">
-        <v>-1160</v>
-      </c>
-      <c r="H32">
-        <v>-400</v>
-      </c>
-      <c r="I32">
-        <v>-410</v>
-      </c>
-      <c r="J32">
-        <v>2428</v>
-      </c>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E33">
-        <v>-366</v>
-      </c>
-      <c r="F33">
-        <v>1619</v>
-      </c>
-      <c r="G33">
-        <v>-360</v>
-      </c>
-      <c r="H33">
-        <v>20</v>
-      </c>
-      <c r="I33">
-        <v>-950</v>
-      </c>
-      <c r="J33">
-        <v>-730</v>
-      </c>
-    </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E34">
-        <v>144</v>
-      </c>
-      <c r="F34">
-        <v>-141</v>
-      </c>
-      <c r="G34">
-        <v>-970</v>
-      </c>
-      <c r="H34">
-        <v>-790</v>
-      </c>
-      <c r="I34">
-        <v>-920</v>
-      </c>
-      <c r="J34">
-        <v>-80</v>
-      </c>
-    </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E35">
-        <v>-1458</v>
-      </c>
-      <c r="F35">
-        <v>-1373</v>
-      </c>
-      <c r="G35">
-        <v>604</v>
-      </c>
-      <c r="H35">
-        <v>2012</v>
-      </c>
-      <c r="I35">
-        <v>130</v>
-      </c>
-      <c r="J35">
-        <v>-350</v>
-      </c>
-    </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E36">
-        <v>28</v>
-      </c>
-      <c r="F36">
-        <v>-86</v>
-      </c>
-      <c r="G36">
-        <v>626</v>
-      </c>
-      <c r="H36">
-        <v>-340</v>
-      </c>
-      <c r="I36">
-        <v>-1040</v>
-      </c>
-      <c r="J36">
-        <v>-1340</v>
-      </c>
-    </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E37">
-        <v>-20</v>
-      </c>
-      <c r="F37">
-        <v>-184</v>
-      </c>
-      <c r="G37">
-        <v>1770</v>
-      </c>
-      <c r="H37">
-        <v>-930</v>
-      </c>
-      <c r="I37">
-        <v>-240</v>
-      </c>
-      <c r="J37">
-        <v>-1250</v>
-      </c>
-    </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E38">
-        <v>-1398</v>
-      </c>
-      <c r="F38">
-        <v>-1118</v>
-      </c>
-      <c r="G38">
-        <v>-1350</v>
-      </c>
-      <c r="H38">
-        <v>920</v>
-      </c>
-      <c r="I38">
-        <v>-1430</v>
-      </c>
-      <c r="J38">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E39">
-        <v>-1426</v>
-      </c>
-      <c r="F39">
-        <v>-1075</v>
-      </c>
-      <c r="G39">
-        <v>-860</v>
-      </c>
-      <c r="H39">
-        <v>640</v>
-      </c>
-      <c r="I39">
-        <v>-1390</v>
-      </c>
-      <c r="J39">
-        <v>-970</v>
-      </c>
-    </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E40">
-        <v>528</v>
-      </c>
-      <c r="F40">
-        <v>1090</v>
-      </c>
-      <c r="G40">
-        <v>900</v>
-      </c>
-      <c r="H40">
-        <v>-130</v>
-      </c>
-      <c r="I40">
-        <v>1666</v>
-      </c>
-      <c r="J40">
-        <v>-540</v>
-      </c>
-    </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E41">
-        <v>-562</v>
-      </c>
-      <c r="F41">
-        <v>-533</v>
-      </c>
-      <c r="G41">
-        <v>2302</v>
-      </c>
-      <c r="H41">
-        <v>-1050</v>
-      </c>
-      <c r="I41">
-        <v>-1700</v>
-      </c>
-      <c r="J41">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E42">
-        <v>-1190</v>
-      </c>
-      <c r="F42">
-        <v>-982</v>
-      </c>
-      <c r="G42">
-        <v>-1170</v>
-      </c>
-      <c r="H42">
-        <v>2322</v>
-      </c>
-      <c r="I42">
-        <v>710</v>
-      </c>
-      <c r="J42">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E43">
-        <v>-748</v>
-      </c>
-      <c r="F43">
-        <v>-870</v>
-      </c>
-      <c r="G43">
-        <v>-1390</v>
-      </c>
-      <c r="H43">
-        <v>-1700</v>
-      </c>
-      <c r="I43">
-        <v>-1160</v>
-      </c>
-      <c r="J43">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E44">
-        <v>430</v>
-      </c>
-      <c r="F44">
-        <v>973</v>
-      </c>
-      <c r="G44">
-        <v>-1170</v>
-      </c>
-      <c r="H44">
-        <v>100</v>
-      </c>
-      <c r="I44">
-        <v>-940</v>
-      </c>
-      <c r="J44">
-        <v>-1100</v>
-      </c>
-    </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E45">
-        <v>-1562</v>
-      </c>
-      <c r="F45">
-        <v>-1442</v>
-      </c>
-      <c r="G45">
-        <v>-310</v>
-      </c>
-      <c r="H45">
-        <v>-1140</v>
-      </c>
-      <c r="I45">
-        <v>-770</v>
-      </c>
-      <c r="J45">
-        <v>-1600</v>
-      </c>
-    </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E46">
-        <v>1630</v>
-      </c>
-      <c r="F46">
-        <v>1094</v>
-      </c>
-      <c r="G46">
-        <v>-280</v>
-      </c>
-      <c r="H46">
-        <v>-530</v>
-      </c>
-      <c r="I46">
-        <v>-600</v>
-      </c>
-      <c r="J46">
-        <v>6270</v>
-      </c>
-    </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E47">
-        <v>-688</v>
-      </c>
-      <c r="F47">
-        <v>-806</v>
-      </c>
-      <c r="G47">
-        <v>-160</v>
-      </c>
-      <c r="H47">
-        <v>-260</v>
-      </c>
-      <c r="I47">
-        <v>680</v>
-      </c>
-      <c r="J47">
-        <v>-340</v>
-      </c>
-    </row>
-    <row r="48" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E48">
-        <v>2498</v>
-      </c>
-      <c r="F48">
-        <v>4957</v>
-      </c>
-      <c r="G48">
-        <v>-910</v>
-      </c>
-      <c r="H48">
-        <v>3272</v>
-      </c>
-      <c r="I48">
-        <v>1892</v>
-      </c>
-      <c r="J48">
-        <v>-1260</v>
-      </c>
-    </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E49">
-        <v>2137</v>
-      </c>
-      <c r="F49">
-        <v>1438</v>
-      </c>
-      <c r="G49">
-        <v>1360</v>
-      </c>
-      <c r="H49">
-        <v>-1360</v>
-      </c>
-      <c r="I49">
-        <v>-890</v>
-      </c>
-      <c r="J49">
-        <v>-80</v>
-      </c>
-    </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E50">
-        <v>1398</v>
-      </c>
-      <c r="F50">
-        <v>891</v>
-      </c>
-      <c r="G50">
-        <v>1646</v>
-      </c>
-      <c r="H50">
-        <v>-1470</v>
-      </c>
-      <c r="I50">
-        <v>-900</v>
-      </c>
-      <c r="J50">
-        <v>-1700</v>
-      </c>
-    </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-      <c r="J51">
-        <v>0</v>
+        <v>-576</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>